<commit_message>
documentation for django car enquiry form
</commit_message>
<xml_diff>
--- a/car_enquiry_form/car_enquiry_data.xlsx
+++ b/car_enquiry_form/car_enquiry_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,6 +553,67 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tata</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Model 2024</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Diesel</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>TamilNadu</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Chandru</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chandru</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>7092312288</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>chandru@gmail.com</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>